<commit_message>
23 Jan 2025 - Initial
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0011418_VerifyTASSupervisorCanMoreThan24hoursForOneDayForAssociatesWithTitleTAGOutsourcedContractor.xlsx
+++ b/TestData/LV_TMTT0011418_VerifyTASSupervisorCanMoreThan24hoursForOneDayForAssociatesWithTitleTAGOutsourcedContractor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269075B0-CDBB-4EBD-A6E4-930D6629CBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6476351B-6BCB-4E87-9436-5D9F2ADD53A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="8" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Project Bend-Bernhard Capital Partners Management-FVA-109081</t>
   </si>
   <si>
-    <t>Project Clear-LucidHealth-FVA-105379</t>
-  </si>
-  <si>
     <t>Christy Skaar</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Time Record Manager</t>
+  </si>
+  <si>
+    <t>Bartush-Cotton Creek Capital Management LLC-FVA-110095</t>
   </si>
 </sst>
 </file>
@@ -813,19 +813,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -842,19 +842,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -870,19 +870,19 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -895,17 +895,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -913,9 +913,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -938,17 +938,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -966,14 +966,14 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -991,9 +991,9 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1019,16 +1019,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1036,9 +1036,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1054,15 +1054,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1070,9 +1070,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>

</xml_diff>